<commit_message>
added excel file with courses and testing
</commit_message>
<xml_diff>
--- a/scheduler-input-draf1.xlsx
+++ b/scheduler-input-draf1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t xml:space="preserve">Conflict Courses</t>
   </si>
@@ -149,7 +149,7 @@
     <t xml:space="preserve">Tuesday / Thursday</t>
   </si>
   <si>
-    <t xml:space="preserve">09:00 / 11:00</t>
+    <t xml:space="preserve">08:00 / 17:30</t>
   </si>
   <si>
     <t xml:space="preserve">ENG205</t>
@@ -164,9 +164,6 @@
     <t xml:space="preserve">Monday / Wednesday</t>
   </si>
   <si>
-    <t xml:space="preserve">13:00 / 14:30</t>
-  </si>
-  <si>
     <t xml:space="preserve">HIST301</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t xml:space="preserve">Dr. Williams</t>
   </si>
   <si>
-    <t xml:space="preserve">14:00 / 15:30</t>
-  </si>
-  <si>
     <t xml:space="preserve">ART202</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t xml:space="preserve">Prof. Lee</t>
   </si>
   <si>
-    <t xml:space="preserve">16:00 / 17:30</t>
-  </si>
-  <si>
     <t xml:space="preserve">PSYC301</t>
   </si>
   <si>
@@ -200,9 +191,6 @@
     <t xml:space="preserve">Dr. Rodriguez</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00 / 11:30</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHEM202</t>
   </si>
   <si>
@@ -212,9 +200,6 @@
     <t xml:space="preserve">Prof. Anderson</t>
   </si>
   <si>
-    <t xml:space="preserve">13:00 / 15:00</t>
-  </si>
-  <si>
     <t xml:space="preserve">PHYS110</t>
   </si>
   <si>
@@ -224,18 +209,12 @@
     <t xml:space="preserve">Dr. Thompson</t>
   </si>
   <si>
-    <t xml:space="preserve">14:00 / 16:00</t>
-  </si>
-  <si>
     <t xml:space="preserve">BUSN301</t>
   </si>
   <si>
     <t xml:space="preserve">Marketing Strategies</t>
   </si>
   <si>
-    <t xml:space="preserve">09:00 / 10:30</t>
-  </si>
-  <si>
     <t xml:space="preserve">LANG202</t>
   </si>
   <si>
@@ -243,6 +222,9 @@
   </si>
   <si>
     <t xml:space="preserve">Prof. Hernandez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friday</t>
   </si>
 </sst>
 </file>
@@ -252,7 +234,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Nimbus Sans"/>
@@ -273,6 +255,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Nimbus Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -317,7 +304,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -327,6 +314,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -350,7 +341,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -511,7 +502,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -563,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>2</v>
@@ -589,7 +580,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>3</v>
@@ -615,7 +606,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>4</v>
@@ -652,68 +643,68 @@
       <c r="G5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>47</v>
+      <c r="H5" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>51</v>
+      <c r="H6" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>55</v>
+      <c r="H7" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>3</v>
@@ -725,73 +716,73 @@
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>59</v>
+      <c r="H8" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>63</v>
+      <c r="H9" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>67</v>
+      <c r="H10" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>3</v>
@@ -808,16 +799,16 @@
       <c r="G11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>70</v>
+      <c r="H11" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>2</v>
@@ -829,13 +820,13 @@
         <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>